<commit_message>
refact + class for OLR
</commit_message>
<xml_diff>
--- a/solutions/Experiment.xlsx
+++ b/solutions/Experiment.xlsx
@@ -485,31 +485,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>2040</v>
       </c>
       <c r="C2" t="n">
-        <v>782.92</v>
+        <v>149092</v>
       </c>
       <c r="D2" t="n">
-        <v>782.92</v>
+        <v>149092</v>
       </c>
       <c r="E2" t="n">
-        <v>-30.6405668316832</v>
+        <v>44.98407253963344</v>
       </c>
       <c r="F2" t="n">
-        <v>1.139934405940594</v>
+        <v>0.2203999800807702</v>
       </c>
       <c r="G2" t="n">
-        <v>5.329070518200751e-14</v>
+        <v>3.694822225952521e-12</v>
       </c>
       <c r="H2" t="n">
-        <v>3.40349970429088e-12</v>
+        <v>2.801243681460619e-10</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9904272862304768</v>
+        <v>0.7560416917044475</v>
       </c>
       <c r="J2" t="n">
-        <v>0.980946209309864</v>
+        <v>0.5715990395953239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>